<commit_message>
Add test_import.csv and test_import.xlsx
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/test_import.xlsx
+++ b/test_import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlienrust/Library/Mobile Documents/com~apple~CloudDocs/KatharosOps/OUTRUN/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12076D33-B67D-EE46-A61F-081167BECFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A830940-E9D2-9D4A-8BAE-E259C152858C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="520" windowWidth="28040" windowHeight="16040" xr2:uid="{AE36E6D8-673B-5F42-884E-62AB76ED4FFE}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="28040" windowHeight="16040" xr2:uid="{AE36E6D8-673B-5F42-884E-62AB76ED4FFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>rsa_id</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>JP Rust</t>
+  </si>
+  <si>
+    <t>id_number</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,18 +444,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>960103</v>
@@ -463,7 +463,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>960108</v>
@@ -471,7 +471,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>940722</v>

</xml_diff>